<commit_message>
update with new results
</commit_message>
<xml_diff>
--- a/Resources/Model_Result_Records.xlsx
+++ b/Resources/Model_Result_Records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/294ca3c137fc4ff4/Documents/PROJECTS/Project4/hockey_project/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20ED0A4E-4DB5-4EBB-AED5-6CF5144438FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E50224D-46BA-49AA-8862-F3C6E6AF2C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7F7B54A-B49A-4109-B2C3-7FB7108ECDF1}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A7F7B54A-B49A-4109-B2C3-7FB7108ECDF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -792,17 +792,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>933901</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200514</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>419158</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB70CFB4-5F26-E19F-D339-2C19BA7E41B8}"/>
+      <xdr:rowOff>409632</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37D11C2B-43B6-1B15-25A6-F0A46FDAB4EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -819,7 +819,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="19840575"/>
-          <a:ext cx="3229426" cy="419158"/>
+          <a:ext cx="3505689" cy="409632"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -837,16 +837,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>981673</xdr:colOff>
+      <xdr:colOff>1029305</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>390580</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A65BB36-5503-D0BB-07D3-EDF817F751DD}"/>
+      <xdr:rowOff>352474</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3F892BF-9B82-88EA-D66E-9668BF58FBD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -863,7 +863,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="20278725"/>
-          <a:ext cx="4286848" cy="390580"/>
+          <a:ext cx="4334480" cy="352474"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1175,7 +1175,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>